<commit_message>
Changes for matrix and demand plots.
</commit_message>
<xml_diff>
--- a/t_c.xlsx
+++ b/t_c.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steinkruger\Documents\GitHub\t\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A26528D9-AB36-41AE-AE73-EA884FCB5383}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5672BB5-DCA4-4831-A1F3-E699E17CBA81}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Poaching Calculation Replicate " sheetId="5" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -170,7 +169,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -196,6 +199,11 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -224,10 +232,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -243,8 +252,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -567,9 +578,9 @@
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -618,13 +629,13 @@
         <v>7</v>
       </c>
       <c r="B3" s="1">
+        <v>90</v>
+      </c>
+      <c r="C3" s="1">
+        <v>60</v>
+      </c>
+      <c r="D3" s="1">
         <v>120</v>
-      </c>
-      <c r="C3" s="1">
-        <v>80</v>
-      </c>
-      <c r="D3" s="1">
-        <v>180</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>5</v>
@@ -991,15 +1002,15 @@
       </c>
       <c r="B21">
         <f>B2*B3*B4</f>
-        <v>3600</v>
+        <v>2700</v>
       </c>
       <c r="C21" s="3">
         <f t="shared" ref="C21:D21" si="2">C2*C3*C4</f>
-        <v>2640</v>
+        <v>1980</v>
       </c>
       <c r="D21" s="3">
         <f t="shared" si="2"/>
-        <v>7200</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" customHeight="1">
@@ -1008,15 +1019,15 @@
       </c>
       <c r="B22">
         <f>B21*B6</f>
-        <v>1890000</v>
+        <v>1417500</v>
       </c>
       <c r="C22" s="3">
         <f t="shared" ref="C22:D22" si="3">C21*C6</f>
-        <v>1188000</v>
+        <v>891000</v>
       </c>
       <c r="D22" s="3">
         <f t="shared" si="3"/>
-        <v>4320000</v>
+        <v>2880000</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1">
@@ -1025,15 +1036,15 @@
       </c>
       <c r="B23" s="3">
         <f>B21*B5</f>
-        <v>108000</v>
+        <v>81000</v>
       </c>
       <c r="C23" s="3">
         <f t="shared" ref="C23:D23" si="4">C21*C5</f>
-        <v>79200</v>
+        <v>59400</v>
       </c>
       <c r="D23" s="3">
         <f t="shared" si="4"/>
-        <v>216000</v>
+        <v>144000</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15" customHeight="1">
@@ -1042,15 +1053,15 @@
       </c>
       <c r="B24">
         <f>B9*(B10*B11*B21+B18)</f>
-        <v>18276654.545454543</v>
+        <v>13956654.545454545</v>
       </c>
       <c r="C24" s="3">
         <f t="shared" ref="C24:D24" si="5">C9*(C10*C11*C21+C18)</f>
-        <v>3832436.3636363638</v>
+        <v>3040436.3636363638</v>
       </c>
       <c r="D24" s="3">
         <f t="shared" si="5"/>
-        <v>87728872.727272734</v>
+        <v>58928872.727272727</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15" customHeight="1">
@@ -1091,34 +1102,34 @@
       <c r="A27" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="15">
         <f>SUM(B22:B26)</f>
-        <v>21581727.27272727</v>
-      </c>
-      <c r="C27" s="3">
+        <v>16762227.272727272</v>
+      </c>
+      <c r="C27" s="15">
         <f t="shared" ref="C27:D27" si="8">SUM(C22:C26)</f>
-        <v>6342645.4545454541</v>
-      </c>
-      <c r="D27" s="3">
+        <v>5233845.4545454551</v>
+      </c>
+      <c r="D27" s="15">
         <f t="shared" si="8"/>
-        <v>93636009.090909109</v>
+        <v>63324009.090909086</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" customHeight="1">
       <c r="A28" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="15">
         <f>B27/B2</f>
-        <v>179847.72727272724</v>
-      </c>
-      <c r="C28" s="3">
+        <v>139685.22727272726</v>
+      </c>
+      <c r="C28" s="15">
         <f t="shared" ref="C28:D28" si="9">C27/C2</f>
-        <v>63426.454545454544</v>
-      </c>
-      <c r="D28" s="3">
+        <v>52338.454545454551</v>
+      </c>
+      <c r="D28" s="15">
         <f t="shared" si="9"/>
-        <v>468180.04545454553</v>
+        <v>316620.04545454541</v>
       </c>
     </row>
   </sheetData>

</xml_diff>